<commit_message>
a general update of data, figures and text
</commit_message>
<xml_diff>
--- a/Experiment 1/original_data/reldiv_exp1_master.xlsx
+++ b/Experiment 1/original_data/reldiv_exp1_master.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10412"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jcommon/OneDrive - University of Exeter/Data/Relative_diversity/Experiment 1/original_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jcommon/Documents/OneDrive - University of Exeter/Data/Relative_diversity/Experiment 1/original_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="934" documentId="11_B95A2EAF11EACBA707868FCEE52BF4D97D23B020" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B543931B-391F-4845-A4A1-5145BBEE5909}"/>
+  <xr:revisionPtr revIDLastSave="937" documentId="11_B95A2EAF11EACBA707868FCEE52BF4D97D23B020" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{B777B498-E0B9-744F-B45F-8F014B6C5CE9}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,18 +16,12 @@
     <sheet name="dynamics_master.csv" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">dynamics_master.csv!$B$1:$B$130</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">dynamics_master.csv!$J$1:$J$130</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -623,11 +617,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:W130"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="94" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L131" sqref="L131"/>
+      <pane ySplit="2" topLeftCell="A124" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J2" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -684,7 +679,7 @@
       </c>
       <c r="W1" s="31"/>
     </row>
-    <row r="2" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>34</v>
       </c>
@@ -755,7 +750,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10">
         <v>3</v>
       </c>
@@ -824,7 +819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10">
         <v>3</v>
       </c>
@@ -893,7 +888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="10">
         <v>3</v>
       </c>
@@ -962,7 +957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10">
         <v>3</v>
       </c>
@@ -1031,7 +1026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="10">
         <v>3</v>
       </c>
@@ -1100,7 +1095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10">
         <v>3</v>
       </c>
@@ -1169,7 +1164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="10">
         <v>3</v>
       </c>
@@ -1238,7 +1233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="10">
         <v>3</v>
       </c>
@@ -1307,7 +1302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="10">
         <v>3</v>
       </c>
@@ -1388,7 +1383,7 @@
         <v>-0.18645677452751475</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="10">
         <v>3</v>
       </c>
@@ -1469,7 +1464,7 @@
         <v>-0.78295013326541252</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="10">
         <v>3</v>
       </c>
@@ -1550,7 +1545,7 @@
         <v>0.18540624310241371</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="10">
         <v>3</v>
       </c>
@@ -1631,7 +1626,7 @@
         <v>-0.26626788940476942</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="10">
         <v>3</v>
       </c>
@@ -1712,7 +1707,7 @@
         <v>0.20605448243312452</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="10">
         <v>3</v>
       </c>
@@ -1793,7 +1788,7 @@
         <v>-0.24987747321659981</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="10">
         <v>3</v>
       </c>
@@ -1874,7 +1869,7 @@
         <v>-0.16749108729376361</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="10">
         <v>3</v>
       </c>
@@ -1955,7 +1950,7 @@
         <v>-0.30466428031907533</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="10">
         <v>3</v>
       </c>
@@ -2036,7 +2031,7 @@
         <v>-0.63745196641680379</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="10">
         <v>3</v>
       </c>
@@ -2117,7 +2112,7 @@
         <v>-0.48811663902112568</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="10">
         <v>3</v>
       </c>
@@ -2198,7 +2193,7 @@
         <v>-0.15064413684320177</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="10">
         <v>3</v>
       </c>
@@ -2279,7 +2274,7 @@
         <v>-0.33579210192319309</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="10">
         <v>3</v>
       </c>
@@ -2360,7 +2355,7 @@
         <v>-0.25181197299379954</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="10">
         <v>3</v>
       </c>
@@ -2441,7 +2436,7 @@
         <v>0.12493873660829991</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="10">
         <v>3</v>
       </c>
@@ -2522,7 +2517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="10">
         <v>3</v>
       </c>
@@ -2603,7 +2598,7 @@
         <v>-6.6946789630613179E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="10">
         <v>3</v>
       </c>
@@ -2684,7 +2679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="10">
         <v>3</v>
       </c>
@@ -2763,7 +2758,7 @@
         <v>0.90308998699194376</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="10">
         <v>3</v>
       </c>
@@ -2824,7 +2819,7 @@
         <v>410000000</v>
       </c>
       <c r="S29">
-        <f t="shared" ref="S28:S33" si="13">LOG(O29/O21)</f>
+        <f t="shared" ref="S29:S33" si="13">LOG(O29/O21)</f>
         <v>-0.23312976002604538</v>
       </c>
       <c r="T29">
@@ -2832,7 +2827,7 @@
         <v>-0.42596873227228116</v>
       </c>
       <c r="U29">
-        <f t="shared" ref="U28:U34" si="14">LOG(Q29/Q21)</f>
+        <f t="shared" ref="U29:U34" si="14">LOG(Q29/Q21)</f>
         <v>9.691001300805642E-2</v>
       </c>
       <c r="V29">
@@ -2844,7 +2839,7 @@
         <v>0.52287874528033762</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="10">
         <v>3</v>
       </c>
@@ -2925,7 +2920,7 @@
         <v>0.47712125471966244</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="10">
         <v>3</v>
       </c>
@@ -3006,7 +3001,7 @@
         <v>-0.25527250510330601</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="10">
         <v>3</v>
       </c>
@@ -3087,7 +3082,7 @@
         <v>0.3010299956639812</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="10">
         <v>3</v>
       </c>
@@ -3168,7 +3163,7 @@
         <v>0.12493873660829991</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="10">
         <v>3</v>
       </c>
@@ -3249,7 +3244,7 @@
         <v>-0.3010299956639812</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="10">
         <v>6</v>
       </c>
@@ -3318,7 +3313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="10">
         <v>6</v>
       </c>
@@ -3387,7 +3382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="10">
         <v>6</v>
       </c>
@@ -3456,7 +3451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="10">
         <v>6</v>
       </c>
@@ -3525,7 +3520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="10">
         <v>6</v>
       </c>
@@ -3594,7 +3589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="10">
         <v>6</v>
       </c>
@@ -3663,7 +3658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="10">
         <v>6</v>
       </c>
@@ -3732,7 +3727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="10">
         <v>6</v>
       </c>
@@ -3801,7 +3796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="10">
         <v>6</v>
       </c>
@@ -3882,7 +3877,7 @@
         <v>-0.35218251811136247</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="10">
         <v>6</v>
       </c>
@@ -3963,7 +3958,7 @@
         <v>0.11041248341170329</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="10">
         <v>6</v>
       </c>
@@ -4044,7 +4039,7 @@
         <v>0.18184358794477262</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="10">
         <v>6</v>
       </c>
@@ -4125,7 +4120,7 @@
         <v>-0.21573182480667441</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="10">
         <v>6</v>
       </c>
@@ -4206,7 +4201,7 @@
         <v>0.37238590419964934</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="10">
         <v>6</v>
       </c>
@@ -4287,7 +4282,7 @@
         <v>0.11960990310323272</v>
       </c>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="10">
         <v>6</v>
       </c>
@@ -4368,7 +4363,7 @@
         <v>-0.89085553057493194</v>
       </c>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="10">
         <v>6</v>
       </c>
@@ -4449,7 +4444,7 @@
         <v>0.13127891463931896</v>
       </c>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="10">
         <v>6</v>
       </c>
@@ -4530,7 +4525,7 @@
         <v>-0.24073409377673016</v>
       </c>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="10">
         <v>6</v>
       </c>
@@ -4611,7 +4606,7 @@
         <v>-0.46943442605337143</v>
       </c>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="10">
         <v>6</v>
       </c>
@@ -4692,7 +4687,7 @@
         <v>0.25181197299379959</v>
       </c>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="10">
         <v>6</v>
       </c>
@@ -4773,7 +4768,7 @@
         <v>-0.25390140852043808</v>
       </c>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="10">
         <v>6</v>
       </c>
@@ -4854,7 +4849,7 @@
         <v>0.15237698495523955</v>
       </c>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="10">
         <v>6</v>
       </c>
@@ -4935,7 +4930,7 @@
         <v>0.24763636144400536</v>
       </c>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="10">
         <v>6</v>
       </c>
@@ -5016,7 +5011,7 @@
         <v>0.6020599913279624</v>
       </c>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="10">
         <v>6</v>
       </c>
@@ -5097,7 +5092,7 @@
         <v>-0.47924494834951792</v>
       </c>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="10">
         <v>6</v>
       </c>
@@ -5177,7 +5172,7 @@
         <v>-7.0225073409978513</v>
       </c>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="10">
         <v>6</v>
       </c>
@@ -5258,7 +5253,7 @@
         <v>0.6020599913279624</v>
       </c>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="10">
         <v>6</v>
       </c>
@@ -5339,7 +5334,7 @@
         <v>6.6946789630613235E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="10">
         <v>6</v>
       </c>
@@ -5420,7 +5415,7 @@
         <v>-0.15678610386029462</v>
       </c>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="10">
         <v>6</v>
       </c>
@@ -5501,7 +5496,7 @@
         <v>-0.524762889154889</v>
       </c>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="10">
         <v>6</v>
       </c>
@@ -5582,7 +5577,7 @@
         <v>0.12210944658943568</v>
       </c>
     </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="10">
         <v>6</v>
       </c>
@@ -5663,7 +5658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="10">
         <v>6</v>
       </c>
@@ -5744,7 +5739,7 @@
         <v>-6.8457380655851718E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="16">
         <v>12</v>
       </c>
@@ -5811,7 +5806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="16">
         <v>12</v>
       </c>
@@ -5878,7 +5873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="16">
         <v>12</v>
       </c>
@@ -5945,7 +5940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="16">
         <v>12</v>
       </c>
@@ -6012,7 +6007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="16">
         <v>12</v>
       </c>
@@ -6079,7 +6074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="16">
         <v>12</v>
       </c>
@@ -6146,7 +6141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="16">
         <v>12</v>
       </c>
@@ -6213,7 +6208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="16">
         <v>12</v>
       </c>
@@ -6280,7 +6275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="16">
         <v>12</v>
       </c>
@@ -6361,7 +6356,7 @@
         <v>-0.22184874961635614</v>
       </c>
     </row>
-    <row r="76" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="16">
         <v>12</v>
       </c>
@@ -6442,7 +6437,7 @@
         <v>-0.70376888721778741</v>
       </c>
     </row>
-    <row r="77" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="16">
         <v>12</v>
       </c>
@@ -6523,7 +6518,7 @@
         <v>0.13917917572291016</v>
       </c>
     </row>
-    <row r="78" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="16">
         <v>12</v>
       </c>
@@ -6604,7 +6599,7 @@
         <v>0.39120662601306888</v>
       </c>
     </row>
-    <row r="79" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="16">
         <v>12</v>
       </c>
@@ -6685,7 +6680,7 @@
         <v>3.9508541283673537E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="16">
         <v>12</v>
       </c>
@@ -6766,7 +6761,7 @@
         <v>0.15838741645359677</v>
       </c>
     </row>
-    <row r="81" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="16">
         <v>12</v>
       </c>
@@ -6847,7 +6842,7 @@
         <v>-0.140178703165037</v>
       </c>
     </row>
-    <row r="82" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="16">
         <v>12</v>
       </c>
@@ -6928,7 +6923,7 @@
         <v>0.23691249605223241</v>
       </c>
     </row>
-    <row r="83" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="16">
         <v>12</v>
       </c>
@@ -7009,7 +7004,7 @@
         <v>0.39794000867203771</v>
       </c>
     </row>
-    <row r="84" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="16">
         <v>12</v>
       </c>
@@ -7090,7 +7085,7 @@
         <v>0.32389287862348548</v>
       </c>
     </row>
-    <row r="85" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="16">
         <v>12</v>
       </c>
@@ -7171,7 +7166,7 @@
         <v>0.49485002168009401</v>
       </c>
     </row>
-    <row r="86" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="16">
         <v>12</v>
       </c>
@@ -7252,7 +7247,7 @@
         <v>-0.46584024430997339</v>
       </c>
     </row>
-    <row r="87" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="16">
         <v>12</v>
       </c>
@@ -7333,7 +7328,7 @@
         <v>-0.63682209758717434</v>
       </c>
     </row>
-    <row r="88" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="16">
         <v>12</v>
       </c>
@@ -7414,7 +7409,7 @@
         <v>-6.7117670798233164E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="16">
         <v>12</v>
       </c>
@@ -7495,7 +7490,7 @@
         <v>0.89510011283020563</v>
       </c>
     </row>
-    <row r="90" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="16">
         <v>12</v>
       </c>
@@ -7576,7 +7571,7 @@
         <v>-6.7352104155508769E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="16">
         <v>12</v>
       </c>
@@ -7656,7 +7651,7 @@
         <v>-7</v>
       </c>
     </row>
-    <row r="92" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="16">
         <v>12</v>
       </c>
@@ -7737,7 +7732,7 @@
         <v>0.79005047368335135</v>
       </c>
     </row>
-    <row r="93" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="16">
         <v>12</v>
       </c>
@@ -7818,7 +7813,7 @@
         <v>-9.691001300805635E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="16">
         <v>12</v>
       </c>
@@ -7898,7 +7893,7 @@
         <v>-6.0222763947111524</v>
       </c>
     </row>
-    <row r="95" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="16">
         <v>12</v>
       </c>
@@ -7979,7 +7974,7 @@
         <v>0.26443619338752489</v>
       </c>
     </row>
-    <row r="96" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="16">
         <v>12</v>
       </c>
@@ -8060,7 +8055,7 @@
         <v>-0.49428927985667642</v>
       </c>
     </row>
-    <row r="97" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="16">
         <v>12</v>
       </c>
@@ -8141,7 +8136,7 @@
         <v>0.7433891441244318</v>
       </c>
     </row>
-    <row r="98" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="16">
         <v>12</v>
       </c>
@@ -8221,7 +8216,7 @@
         <v>-7.5753257380807177</v>
       </c>
     </row>
-    <row r="99" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="8">
         <v>24</v>
       </c>
@@ -8290,7 +8285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="8">
         <v>24</v>
       </c>
@@ -8359,7 +8354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="8">
         <v>24</v>
       </c>
@@ -8428,7 +8423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="8">
         <v>24</v>
       </c>
@@ -8497,7 +8492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="8">
         <v>24</v>
       </c>
@@ -8566,7 +8561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="8">
         <v>24</v>
       </c>
@@ -8635,7 +8630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="8">
         <v>24</v>
       </c>
@@ -8704,7 +8699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="8">
         <v>24</v>
       </c>
@@ -8773,7 +8768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="8">
         <v>24</v>
       </c>
@@ -8854,7 +8849,7 @@
         <v>-0.35427550761720639</v>
       </c>
     </row>
-    <row r="108" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="8">
         <v>24</v>
       </c>
@@ -8935,7 +8930,7 @@
         <v>-0.34845464559211914</v>
       </c>
     </row>
-    <row r="109" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="8">
         <v>24</v>
       </c>
@@ -9016,7 +9011,7 @@
         <v>-0.2606013386083732</v>
       </c>
     </row>
-    <row r="110" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="8">
         <v>24</v>
       </c>
@@ -9097,7 +9092,7 @@
         <v>-0.38154959248386833</v>
       </c>
     </row>
-    <row r="111" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="8">
         <v>24</v>
       </c>
@@ -9178,7 +9173,7 @@
         <v>-0.59522056679765711</v>
       </c>
     </row>
-    <row r="112" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="8">
         <v>24</v>
       </c>
@@ -9259,7 +9254,7 @@
         <v>-0.29056456198581637</v>
       </c>
     </row>
-    <row r="113" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="8">
         <v>24</v>
       </c>
@@ -9340,7 +9335,7 @@
         <v>-5.1152522447381443E-2</v>
       </c>
     </row>
-    <row r="114" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="8">
         <v>24</v>
       </c>
@@ -9421,7 +9416,7 @@
         <v>-0.10563358141291301</v>
       </c>
     </row>
-    <row r="115" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="8">
         <v>24</v>
       </c>
@@ -9502,7 +9497,7 @@
         <v>-0.11539341870206954</v>
       </c>
     </row>
-    <row r="116" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="8">
         <v>24</v>
       </c>
@@ -9583,7 +9578,7 @@
         <v>-6.2147906748844406E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="8">
         <v>24</v>
       </c>
@@ -9664,7 +9659,7 @@
         <v>-0.92081875395237534</v>
       </c>
     </row>
-    <row r="118" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="8">
         <v>24</v>
       </c>
@@ -9745,7 +9740,7 @@
         <v>0.30102999566398125</v>
       </c>
     </row>
-    <row r="119" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" s="8">
         <v>24</v>
       </c>
@@ -9826,7 +9821,7 @@
         <v>0.46375729316168091</v>
       </c>
     </row>
-    <row r="120" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="8">
         <v>24</v>
       </c>
@@ -9907,7 +9902,7 @@
         <v>-0.19629464514396799</v>
       </c>
     </row>
-    <row r="121" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="8">
         <v>24</v>
       </c>
@@ -9988,7 +9983,7 @@
         <v>0.60205999132796206</v>
       </c>
     </row>
-    <row r="122" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="8">
         <v>24</v>
       </c>
@@ -10069,7 +10064,7 @@
         <v>-0.25632026069449987</v>
       </c>
     </row>
-    <row r="123" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="8">
         <v>24</v>
       </c>
@@ -10311,7 +10306,7 @@
         <v>-6.5228787452803374</v>
       </c>
     </row>
-    <row r="126" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" s="8">
         <v>24</v>
       </c>
@@ -10391,7 +10386,7 @@
         <v>-6.7727562184969372</v>
       </c>
     </row>
-    <row r="127" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" s="8">
         <v>24</v>
       </c>
@@ -10472,7 +10467,7 @@
         <v>0.43933269383026252</v>
       </c>
     </row>
-    <row r="128" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" s="8">
         <v>24</v>
       </c>
@@ -10715,8 +10710,14 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:B130" xr:uid="{B9A78A06-7CCB-4E4B-9227-CB1B19383DCE}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:W130">
+  <autoFilter ref="J1:J130" xr:uid="{2287D050-63EA-CE47-AC5C-3C78A2026166}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="0"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <sortState ref="A3:W130">
     <sortCondition ref="A2"/>
   </sortState>
   <mergeCells count="6">

</xml_diff>